<commit_message>
test as of 04/15/2017 (including SE domain)
</commit_message>
<xml_diff>
--- a/Updated/opencdisc-report-SDTM.xlsx
+++ b/Updated/opencdisc-report-SDTM.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2209" uniqueCount="1343">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1948" uniqueCount="1294">
   <si>
     <t>Pinnacle 21 ID</t>
   </si>
@@ -3809,238 +3809,91 @@
     <t>Values</t>
   </si>
   <si>
+    <t>Pinnacle 21 Validator Report</t>
+  </si>
+  <si>
+    <t>Configuration: C:\Users\peternew\Documents\Utilities\pinnacle21-community\components\config\SDTM 3.2.xml</t>
+  </si>
+  <si>
+    <t>Define.xml: C:\Users\peternew\Documents\Utilities\pinnacle21-community</t>
+  </si>
+  <si>
+    <t>Generated: 2016-08-03T11:10:30</t>
+  </si>
+  <si>
+    <t>CDISC CT Version: 2016-06-26</t>
+  </si>
+  <si>
+    <t>UNII Version: 2016-07-06</t>
+  </si>
+  <si>
+    <t>NDF-RT Version: 2016-07-05</t>
+  </si>
+  <si>
+    <t>Software Version: 2.1.2</t>
+  </si>
+  <si>
+    <t>Issue Summary</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>Found</t>
+  </si>
+  <si>
+    <t>Processed Sources</t>
+  </si>
+  <si>
+    <t>Label</t>
+  </si>
+  <si>
+    <t>Class</t>
+  </si>
+  <si>
+    <t>Records</t>
+  </si>
+  <si>
+    <t>Rejects</t>
+  </si>
+  <si>
+    <t>Errors</t>
+  </si>
+  <si>
+    <t>Warnings</t>
+  </si>
+  <si>
+    <t>Notices</t>
+  </si>
+  <si>
     <t>GLOBAL</t>
   </si>
   <si>
-    <t>DOMAIN</t>
-  </si>
-  <si>
-    <t>AE</t>
-  </si>
-  <si>
-    <t>LB</t>
-  </si>
-  <si>
-    <t>EX</t>
-  </si>
-  <si>
-    <t>SE</t>
+    <t>Global Metadata</t>
+  </si>
+  <si>
+    <t>--</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Unprocessed Sources</t>
+  </si>
+  <si>
+    <t>Reason</t>
   </si>
   <si>
     <t>DM</t>
   </si>
   <si>
-    <t>ARMCD, ACTARMCD</t>
-  </si>
-  <si>
-    <t>Xan_Hi, Xan_Lo</t>
-  </si>
-  <si>
-    <t>DS</t>
-  </si>
-  <si>
-    <t>VARIABLE</t>
-  </si>
-  <si>
-    <t>VISIT</t>
-  </si>
-  <si>
-    <t>VISITNUM</t>
-  </si>
-  <si>
-    <t>DSDY</t>
-  </si>
-  <si>
-    <t>SUB:RFSTDTC, DSDY, DSDTC</t>
-  </si>
-  <si>
-    <t>2013-07-22, 12, 2013-08-03</t>
-  </si>
-  <si>
-    <t>Incorrect value for DSDY variable</t>
-  </si>
-  <si>
-    <t>TS</t>
-  </si>
-  <si>
-    <t>TSPARM</t>
-  </si>
-  <si>
-    <t>Age Group</t>
-  </si>
-  <si>
-    <t>TSPARM value not found in 'Trial Summary Parameter Test Name' extensible codelist</t>
-  </si>
-  <si>
-    <t>TSPARMCD</t>
-  </si>
-  <si>
-    <t>AGESPAN</t>
-  </si>
-  <si>
-    <t>TSPARMCD value not found in 'Trial Summary Parameter Test Code' extensible codelist</t>
-  </si>
-  <si>
-    <t>VS</t>
-  </si>
-  <si>
-    <t>EPOCH</t>
-  </si>
-  <si>
-    <t>Pinnacle 21 Validator Report</t>
-  </si>
-  <si>
-    <t>Configuration: C:\Users\peternew\Documents\Utilities\pinnacle21-community\components\config\SDTM 3.2.xml</t>
-  </si>
-  <si>
-    <t>Define.xml: C:\Users\peternew\Documents\Utilities\pinnacle21-community</t>
-  </si>
-  <si>
-    <t>Generated: 2017-04-14T14:41:25</t>
-  </si>
-  <si>
-    <t>CDISC CT Version: 2016-06-26</t>
-  </si>
-  <si>
-    <t>UNII Version: 2016-07-06</t>
-  </si>
-  <si>
-    <t>NDF-RT Version: 2016-07-05</t>
-  </si>
-  <si>
-    <t>Software Version: 2.1.2</t>
-  </si>
-  <si>
-    <t>Issue Summary</t>
-  </si>
-  <si>
-    <t>Source</t>
-  </si>
-  <si>
-    <t>Found</t>
-  </si>
-  <si>
-    <t>Processed Sources</t>
-  </si>
-  <si>
-    <t>Label</t>
-  </si>
-  <si>
-    <t>Class</t>
-  </si>
-  <si>
-    <t>Records</t>
-  </si>
-  <si>
-    <t>Rejects</t>
-  </si>
-  <si>
-    <t>Errors</t>
-  </si>
-  <si>
-    <t>Warnings</t>
-  </si>
-  <si>
-    <t>Notices</t>
-  </si>
-  <si>
-    <t>Global Metadata</t>
-  </si>
-  <si>
-    <t>--</t>
-  </si>
-  <si>
     <t>Demographics</t>
   </si>
   <si>
     <t>SPECIAL PURPOSE</t>
   </si>
   <si>
-    <t>dm.xpt</t>
-  </si>
-  <si>
-    <t>Disposition</t>
-  </si>
-  <si>
-    <t>EVENTS</t>
-  </si>
-  <si>
-    <t>ds.xpt</t>
-  </si>
-  <si>
-    <t>SUPPDM</t>
-  </si>
-  <si>
-    <t>Supplemental Qualifiers</t>
-  </si>
-  <si>
-    <t>RELATIONSHIP</t>
-  </si>
-  <si>
-    <t>suppdm.xpt</t>
-  </si>
-  <si>
-    <t>TA</t>
-  </si>
-  <si>
-    <t>Trial Arms</t>
-  </si>
-  <si>
-    <t>TRIAL DESIGN</t>
-  </si>
-  <si>
-    <t>ta.xpt</t>
-  </si>
-  <si>
-    <t>TE</t>
-  </si>
-  <si>
-    <t>Trial Elements</t>
-  </si>
-  <si>
-    <t>te.xpt</t>
-  </si>
-  <si>
-    <t>TI</t>
-  </si>
-  <si>
-    <t>Trial Inclusion/Exclusion Criteria</t>
-  </si>
-  <si>
-    <t>ti.xpt</t>
-  </si>
-  <si>
-    <t>Trial Summary</t>
-  </si>
-  <si>
-    <t>ts.xpt</t>
-  </si>
-  <si>
-    <t>TV</t>
-  </si>
-  <si>
-    <t>Trial Visits</t>
-  </si>
-  <si>
-    <t>tv.xpt</t>
-  </si>
-  <si>
-    <t>Vital Signs</t>
-  </si>
-  <si>
-    <t>FINDINGS</t>
-  </si>
-  <si>
-    <t>vs.xpt</t>
-  </si>
-  <si>
-    <t>Total</t>
-  </si>
-  <si>
-    <t>Unprocessed Sources</t>
-  </si>
-  <si>
-    <t>Reason</t>
+    <t>Validation Aborted</t>
   </si>
   <si>
     <t>Grand Total</t>
@@ -4285,48 +4138,48 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="2">
-        <v>1290</v>
+        <v>1264</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="3">
-        <v>1291</v>
+        <v>1265</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="3">
-        <v>1292</v>
+        <v>1266</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="3">
-        <v>1293</v>
+        <v>1267</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="3">
-        <v>1294</v>
+        <v>1268</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="3">
-        <v>1295</v>
+        <v>1269</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="3">
-        <v>1296</v>
+        <v>1270</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="3">
-        <v>1297</v>
+        <v>1271</v>
       </c>
     </row>
     <row r="10"/>
     <row r="11">
       <c r="A11" t="s" s="4">
-        <v>1301</v>
+        <v>1275</v>
       </c>
     </row>
     <row r="12">
@@ -4334,45 +4187,45 @@
         <v>1259</v>
       </c>
       <c r="B12" t="s" s="5">
-        <v>1302</v>
+        <v>1276</v>
       </c>
       <c r="C12" t="s" s="5">
-        <v>1303</v>
+        <v>1277</v>
       </c>
       <c r="D12" t="s" s="5">
-        <v>1299</v>
+        <v>1273</v>
       </c>
       <c r="E12" t="s" s="5">
-        <v>1304</v>
+        <v>1278</v>
       </c>
       <c r="F12" t="s" s="12">
-        <v>1305</v>
+        <v>1279</v>
       </c>
       <c r="G12" t="s" s="15">
-        <v>1306</v>
+        <v>1280</v>
       </c>
       <c r="H12" t="s" s="18">
-        <v>1307</v>
+        <v>1281</v>
       </c>
       <c r="I12" t="s" s="21">
-        <v>1308</v>
+        <v>1282</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="9">
-        <v>1264</v>
+        <v>1283</v>
       </c>
       <c r="B13" t="s" s="9">
-        <v>1309</v>
+        <v>1284</v>
       </c>
       <c r="C13" t="s" s="9">
-        <v>1310</v>
+        <v>1285</v>
       </c>
       <c r="D13" t="s" s="9">
-        <v>1310</v>
+        <v>1285</v>
       </c>
       <c r="E13" t="s" s="9">
-        <v>1310</v>
+        <v>1285</v>
       </c>
       <c r="F13" t="n" s="9">
         <v>0.0</v>
@@ -4381,370 +4234,136 @@
         <v>0.0</v>
       </c>
       <c r="H13" t="n" s="9">
-        <v>4.0</v>
+        <v>0.0</v>
       </c>
       <c r="I13" t="n" s="9">
         <v>0.0</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="s" s="8">
-        <v>1270</v>
-      </c>
-      <c r="B14" t="s" s="8">
-        <v>1311</v>
-      </c>
-      <c r="C14" t="s" s="8">
-        <v>1312</v>
-      </c>
-      <c r="D14" t="s" s="8">
-        <v>1313</v>
-      </c>
-      <c r="E14" t="n" s="8">
-        <v>306.0</v>
-      </c>
-      <c r="F14" t="n" s="8">
+      <c r="A14" t="s" s="7">
+        <v>1286</v>
+      </c>
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="10" t="n">
         <v>0.0</v>
       </c>
-      <c r="G14" t="n" s="8">
+      <c r="F14" s="13" t="n">
         <v>0.0</v>
       </c>
-      <c r="H14" t="n" s="8">
-        <v>12.0</v>
-      </c>
-      <c r="I14" t="n" s="8">
+      <c r="G14" s="16" t="n">
         <v>0.0</v>
       </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="s" s="9">
-        <v>1273</v>
-      </c>
-      <c r="B15" t="s" s="9">
-        <v>1314</v>
-      </c>
-      <c r="C15" t="s" s="9">
-        <v>1315</v>
-      </c>
-      <c r="D15" t="s" s="9">
-        <v>1316</v>
-      </c>
-      <c r="E15" t="n" s="9">
-        <v>596.0</v>
-      </c>
-      <c r="F15" t="n" s="9">
+      <c r="H14" s="19" t="n">
         <v>0.0</v>
       </c>
-      <c r="G15" t="n" s="9">
+      <c r="I14" s="22" t="n">
         <v>0.0</v>
       </c>
-      <c r="H15" t="n" s="9">
-        <v>4.0</v>
-      </c>
-      <c r="I15" t="n" s="9">
+    </row>
+    <row r="15"/>
+    <row r="16">
+      <c r="A16" t="s" s="4">
+        <v>1287</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s" s="5">
+        <v>1259</v>
+      </c>
+      <c r="B17" t="s" s="5">
+        <v>1276</v>
+      </c>
+      <c r="C17" t="s" s="5">
+        <v>1277</v>
+      </c>
+      <c r="D17" t="s" s="5">
+        <v>1288</v>
+      </c>
+      <c r="F17" t="s" s="12">
+        <v>1279</v>
+      </c>
+      <c r="G17" t="s" s="15">
+        <v>1280</v>
+      </c>
+      <c r="H17" t="s" s="18">
+        <v>1281</v>
+      </c>
+      <c r="I17" t="s" s="21">
+        <v>1282</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s" s="9">
+        <v>1289</v>
+      </c>
+      <c r="B18" t="s" s="9">
+        <v>1290</v>
+      </c>
+      <c r="C18" t="s" s="9">
+        <v>1291</v>
+      </c>
+      <c r="D18" t="s" s="9">
+        <v>1292</v>
+      </c>
+      <c r="E18" s="9"/>
+      <c r="F18" t="n" s="9">
         <v>0.0</v>
       </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="s" s="8">
-        <v>1317</v>
-      </c>
-      <c r="B16" t="s" s="8">
-        <v>1318</v>
-      </c>
-      <c r="C16" t="s" s="8">
-        <v>1319</v>
-      </c>
-      <c r="D16" t="s" s="8">
-        <v>1320</v>
-      </c>
-      <c r="E16" t="n" s="8">
-        <v>1197.0</v>
-      </c>
-      <c r="F16" t="n" s="8">
+      <c r="G18" t="n" s="9">
         <v>0.0</v>
       </c>
-      <c r="G16" t="n" s="8">
+      <c r="H18" t="n" s="9">
         <v>0.0</v>
       </c>
-      <c r="H16" t="n" s="8">
+      <c r="I18" t="n" s="9">
         <v>0.0</v>
       </c>
-      <c r="I16" t="n" s="8">
+    </row>
+    <row r="19">
+      <c r="A19" t="s" s="7">
+        <v>1286</v>
+      </c>
+      <c r="B19" s="7"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="13" t="n">
         <v>0.0</v>
       </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="s" s="9">
-        <v>1321</v>
-      </c>
-      <c r="B17" t="s" s="9">
-        <v>1322</v>
-      </c>
-      <c r="C17" t="s" s="9">
-        <v>1323</v>
-      </c>
-      <c r="D17" t="s" s="9">
-        <v>1324</v>
-      </c>
-      <c r="E17" t="n" s="9">
-        <v>11.0</v>
-      </c>
-      <c r="F17" t="n" s="9">
+      <c r="G19" s="16" t="n">
         <v>0.0</v>
       </c>
-      <c r="G17" t="n" s="9">
+      <c r="H19" s="19" t="n">
         <v>0.0</v>
       </c>
-      <c r="H17" t="n" s="9">
+      <c r="I19" s="22" t="n">
         <v>0.0</v>
       </c>
-      <c r="I17" t="n" s="9">
+    </row>
+    <row r="20"/>
+    <row r="21">
+      <c r="A21" t="s" s="7">
+        <v>1293</v>
+      </c>
+      <c r="B21" s="7"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="10" t="n">
         <v>0.0</v>
       </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="s" s="8">
-        <v>1325</v>
-      </c>
-      <c r="B18" t="s" s="8">
-        <v>1326</v>
-      </c>
-      <c r="C18" t="s" s="8">
-        <v>1323</v>
-      </c>
-      <c r="D18" t="s" s="8">
-        <v>1327</v>
-      </c>
-      <c r="E18" t="n" s="8">
-        <v>7.0</v>
-      </c>
-      <c r="F18" t="n" s="8">
+      <c r="F21" s="13" t="n">
         <v>0.0</v>
       </c>
-      <c r="G18" t="n" s="8">
+      <c r="G21" s="16" t="n">
         <v>0.0</v>
       </c>
-      <c r="H18" t="n" s="8">
+      <c r="H21" s="19" t="n">
         <v>0.0</v>
       </c>
-      <c r="I18" t="n" s="8">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="s" s="9">
-        <v>1328</v>
-      </c>
-      <c r="B19" t="s" s="9">
-        <v>1329</v>
-      </c>
-      <c r="C19" t="s" s="9">
-        <v>1323</v>
-      </c>
-      <c r="D19" t="s" s="9">
-        <v>1330</v>
-      </c>
-      <c r="E19" t="n" s="9">
-        <v>31.0</v>
-      </c>
-      <c r="F19" t="n" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="G19" t="n" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="H19" t="n" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="I19" t="n" s="9">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="s" s="8">
-        <v>1281</v>
-      </c>
-      <c r="B20" t="s" s="8">
-        <v>1331</v>
-      </c>
-      <c r="C20" t="s" s="8">
-        <v>1323</v>
-      </c>
-      <c r="D20" t="s" s="8">
-        <v>1332</v>
-      </c>
-      <c r="E20" t="n" s="8">
-        <v>48.0</v>
-      </c>
-      <c r="F20" t="n" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="G20" t="n" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="H20" t="n" s="8">
-        <v>4.0</v>
-      </c>
-      <c r="I20" t="n" s="8">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="s" s="9">
-        <v>1333</v>
-      </c>
-      <c r="B21" t="s" s="9">
-        <v>1334</v>
-      </c>
-      <c r="C21" t="s" s="9">
-        <v>1323</v>
-      </c>
-      <c r="D21" t="s" s="9">
-        <v>1335</v>
-      </c>
-      <c r="E21" t="n" s="9">
-        <v>21.0</v>
-      </c>
-      <c r="F21" t="n" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="G21" t="n" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="H21" t="n" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="I21" t="n" s="9">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="s" s="8">
-        <v>1288</v>
-      </c>
-      <c r="B22" t="s" s="8">
-        <v>1336</v>
-      </c>
-      <c r="C22" t="s" s="8">
-        <v>1337</v>
-      </c>
-      <c r="D22" t="s" s="8">
-        <v>1338</v>
-      </c>
-      <c r="E22" t="n" s="8">
-        <v>29643.0</v>
-      </c>
-      <c r="F22" t="n" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="G22" t="n" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="H22" t="n" s="8">
-        <v>1.0</v>
-      </c>
-      <c r="I22" t="n" s="8">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="s" s="7">
-        <v>1339</v>
-      </c>
-      <c r="B23" s="7"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="7"/>
-      <c r="E23" s="10" t="n">
-        <v>31860.0</v>
-      </c>
-      <c r="F23" s="13" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="G23" s="16" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="H23" s="19" t="n">
-        <v>25.0</v>
-      </c>
-      <c r="I23" s="22" t="n">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="24"/>
-    <row r="25">
-      <c r="A25" t="s" s="4">
-        <v>1340</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="s" s="5">
-        <v>1259</v>
-      </c>
-      <c r="B26" t="s" s="5">
-        <v>1302</v>
-      </c>
-      <c r="C26" t="s" s="5">
-        <v>1303</v>
-      </c>
-      <c r="D26" t="s" s="5">
-        <v>1341</v>
-      </c>
-      <c r="F26" t="s" s="12">
-        <v>1305</v>
-      </c>
-      <c r="G26" t="s" s="15">
-        <v>1306</v>
-      </c>
-      <c r="H26" t="s" s="18">
-        <v>1307</v>
-      </c>
-      <c r="I26" t="s" s="21">
-        <v>1308</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="s" s="7">
-        <v>1339</v>
-      </c>
-      <c r="B27" s="7"/>
-      <c r="C27" s="7"/>
-      <c r="D27" s="7"/>
-      <c r="E27" s="7"/>
-      <c r="F27" s="13" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="G27" s="16" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="H27" s="19" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="I27" s="22" t="n">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="28"/>
-    <row r="29">
-      <c r="A29" t="s" s="7">
-        <v>1342</v>
-      </c>
-      <c r="B29" s="7"/>
-      <c r="C29" s="7"/>
-      <c r="D29" s="7"/>
-      <c r="E29" s="10" t="n">
-        <v>31860.0</v>
-      </c>
-      <c r="F29" s="13" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="G29" s="16" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="H29" s="19" t="n">
-        <v>25.0</v>
-      </c>
-      <c r="I29" s="22" t="n">
+      <c r="I21" s="22" t="n">
         <v>0.0</v>
       </c>
     </row>
@@ -4759,8 +4378,9 @@
     <mergeCell ref="A8:I8"/>
     <mergeCell ref="A9:I9"/>
     <mergeCell ref="A11:I11"/>
-    <mergeCell ref="A25:I25"/>
-    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="A16:I16"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="D18:E18"/>
   </mergeCells>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup fitToWidth="1"/>
@@ -4788,53 +4408,53 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="2">
-        <v>1290</v>
+        <v>1264</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="3">
-        <v>1291</v>
+        <v>1265</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="3">
-        <v>1292</v>
+        <v>1266</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="3">
-        <v>1293</v>
+        <v>1267</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="3">
-        <v>1294</v>
+        <v>1268</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="3">
-        <v>1295</v>
+        <v>1269</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="3">
-        <v>1296</v>
+        <v>1270</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="3">
-        <v>1297</v>
+        <v>1271</v>
       </c>
     </row>
     <row r="10"/>
     <row r="11">
       <c r="A11" t="s" s="4">
-        <v>1298</v>
+        <v>1272</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="5">
-        <v>1299</v>
+        <v>1273</v>
       </c>
       <c r="B12" t="s" s="5">
         <v>0</v>
@@ -4849,237 +4469,7 @@
         <v>5</v>
       </c>
       <c r="F12" t="s" s="6">
-        <v>1300</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="11" t="s">
-        <v>1264</v>
-      </c>
-      <c r="B13" s="11"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="11"/>
-    </row>
-    <row r="14">
-      <c r="A14" s="9"/>
-      <c r="B14" t="s" s="25">
-        <v>738</v>
-      </c>
-      <c r="C14" t="s" s="25">
-        <v>739</v>
-      </c>
-      <c r="D14" t="s" s="9">
-        <v>740</v>
-      </c>
-      <c r="E14" t="s" s="20">
-        <v>16</v>
-      </c>
-      <c r="F14" t="n" s="9">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="8"/>
-      <c r="B15" t="s" s="24">
-        <v>742</v>
-      </c>
-      <c r="C15" t="s" s="24">
-        <v>743</v>
-      </c>
-      <c r="D15" t="s" s="8">
-        <v>744</v>
-      </c>
-      <c r="E15" t="s" s="20">
-        <v>16</v>
-      </c>
-      <c r="F15" t="n" s="8">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="9"/>
-      <c r="B16" t="s" s="25">
-        <v>750</v>
-      </c>
-      <c r="C16" t="s" s="25">
-        <v>751</v>
-      </c>
-      <c r="D16" t="s" s="9">
-        <v>752</v>
-      </c>
-      <c r="E16" t="s" s="20">
-        <v>16</v>
-      </c>
-      <c r="F16" t="n" s="9">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="8"/>
-      <c r="B17" t="s" s="24">
-        <v>758</v>
-      </c>
-      <c r="C17" t="s" s="24">
-        <v>759</v>
-      </c>
-      <c r="D17" t="s" s="8">
-        <v>760</v>
-      </c>
-      <c r="E17" t="s" s="20">
-        <v>16</v>
-      </c>
-      <c r="F17" t="n" s="8">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="11" t="s">
-        <v>1270</v>
-      </c>
-      <c r="B18" s="11"/>
-      <c r="C18" s="11"/>
-      <c r="D18" s="11"/>
-      <c r="E18" s="11"/>
-      <c r="F18" s="11"/>
-    </row>
-    <row r="19">
-      <c r="A19" s="9"/>
-      <c r="B19" t="s" s="25">
-        <v>1149</v>
-      </c>
-      <c r="C19" t="s" s="25">
-        <v>1150</v>
-      </c>
-      <c r="D19" t="s" s="9">
-        <v>1151</v>
-      </c>
-      <c r="E19" t="s" s="20">
-        <v>16</v>
-      </c>
-      <c r="F19" t="n" s="9">
-        <v>12.0</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="11" t="s">
-        <v>1273</v>
-      </c>
-      <c r="B20" s="11"/>
-      <c r="C20" s="11"/>
-      <c r="D20" s="11"/>
-      <c r="E20" s="11"/>
-      <c r="F20" s="11"/>
-    </row>
-    <row r="21">
-      <c r="A21" s="9"/>
-      <c r="B21" t="s" s="25">
-        <v>634</v>
-      </c>
-      <c r="C21" t="s" s="25">
-        <v>635</v>
-      </c>
-      <c r="D21" t="s" s="9">
-        <v>636</v>
-      </c>
-      <c r="E21" t="s" s="20">
-        <v>16</v>
-      </c>
-      <c r="F21" t="n" s="9">
-        <v>3.0</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="8"/>
-      <c r="B22" t="s" s="24">
-        <v>666</v>
-      </c>
-      <c r="C22" t="s" s="24">
-        <v>667</v>
-      </c>
-      <c r="D22" t="s" s="8">
-        <v>1280</v>
-      </c>
-      <c r="E22" t="s" s="20">
-        <v>16</v>
-      </c>
-      <c r="F22" t="n" s="8">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="11" t="s">
-        <v>1281</v>
-      </c>
-      <c r="B23" s="11"/>
-      <c r="C23" s="11"/>
-      <c r="D23" s="11"/>
-      <c r="E23" s="11"/>
-      <c r="F23" s="11"/>
-    </row>
-    <row r="24">
-      <c r="A24" s="9"/>
-      <c r="B24" t="s" s="25">
-        <v>12</v>
-      </c>
-      <c r="C24" t="s" s="25">
-        <v>13</v>
-      </c>
-      <c r="D24" t="s" s="9">
-        <v>1284</v>
-      </c>
-      <c r="E24" t="s" s="20">
-        <v>16</v>
-      </c>
-      <c r="F24" t="n" s="9">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" s="8"/>
-      <c r="B25" t="s" s="24">
-        <v>12</v>
-      </c>
-      <c r="C25" t="s" s="24">
-        <v>13</v>
-      </c>
-      <c r="D25" t="s" s="8">
-        <v>1287</v>
-      </c>
-      <c r="E25" t="s" s="20">
-        <v>16</v>
-      </c>
-      <c r="F25" t="n" s="8">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" s="11" t="s">
-        <v>1288</v>
-      </c>
-      <c r="B26" s="11"/>
-      <c r="C26" s="11"/>
-      <c r="D26" s="11"/>
-      <c r="E26" s="11"/>
-      <c r="F26" s="11"/>
-    </row>
-    <row r="27">
-      <c r="A27" s="9"/>
-      <c r="B27" t="s" s="25">
-        <v>634</v>
-      </c>
-      <c r="C27" t="s" s="25">
-        <v>635</v>
-      </c>
-      <c r="D27" t="s" s="9">
-        <v>636</v>
-      </c>
-      <c r="E27" t="s" s="20">
-        <v>16</v>
-      </c>
-      <c r="F27" t="n" s="9">
-        <v>1.0</v>
+        <v>1274</v>
       </c>
     </row>
   </sheetData>
@@ -5093,34 +4483,7 @@
     <mergeCell ref="A8:F8"/>
     <mergeCell ref="A9:F9"/>
     <mergeCell ref="A11:F11"/>
-    <mergeCell ref="A13:F13"/>
-    <mergeCell ref="A18:F18"/>
-    <mergeCell ref="A20:F20"/>
-    <mergeCell ref="A23:F23"/>
-    <mergeCell ref="A26:F26"/>
   </mergeCells>
-  <hyperlinks>
-    <hyperlink location="'Rules'!A184" ref="B14"/>
-    <hyperlink location="'Rules'!A184" ref="C14"/>
-    <hyperlink location="'Rules'!A185" ref="B15"/>
-    <hyperlink location="'Rules'!A185" ref="C15"/>
-    <hyperlink location="'Rules'!A187" ref="B16"/>
-    <hyperlink location="'Rules'!A187" ref="C16"/>
-    <hyperlink location="'Rules'!A189" ref="B17"/>
-    <hyperlink location="'Rules'!A189" ref="C17"/>
-    <hyperlink location="'Rules'!A287" ref="B19"/>
-    <hyperlink location="'Rules'!A287" ref="C19"/>
-    <hyperlink location="'Rules'!A158" ref="B21"/>
-    <hyperlink location="'Rules'!A158" ref="C21"/>
-    <hyperlink location="'Rules'!A166" ref="B22"/>
-    <hyperlink location="'Rules'!A166" ref="C22"/>
-    <hyperlink location="'Rules'!A3" ref="B24"/>
-    <hyperlink location="'Rules'!A3" ref="C24"/>
-    <hyperlink location="'Rules'!A3" ref="B25"/>
-    <hyperlink location="'Rules'!A3" ref="C25"/>
-    <hyperlink location="'Rules'!A158" ref="B27"/>
-    <hyperlink location="'Rules'!A158" ref="C27"/>
-  </hyperlinks>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup fitToWidth="1"/>
 </worksheet>
@@ -5181,703 +4544,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="s" s="8">
-        <v>1264</v>
-      </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" t="s" s="8">
-        <v>1265</v>
-      </c>
-      <c r="E2" t="s" s="8">
-        <v>1266</v>
-      </c>
-      <c r="F2" t="s" s="24">
-        <v>738</v>
-      </c>
-      <c r="G2" t="s" s="24">
-        <v>739</v>
-      </c>
-      <c r="H2" t="s" s="8">
-        <v>740</v>
-      </c>
-      <c r="I2" t="s" s="8">
-        <v>37</v>
-      </c>
-      <c r="J2" t="s" s="8">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s" s="8">
-        <v>1264</v>
-      </c>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" t="s" s="8">
-        <v>1265</v>
-      </c>
-      <c r="E3" t="s" s="8">
-        <v>1267</v>
-      </c>
-      <c r="F3" t="s" s="24">
-        <v>742</v>
-      </c>
-      <c r="G3" t="s" s="24">
-        <v>743</v>
-      </c>
-      <c r="H3" t="s" s="8">
-        <v>744</v>
-      </c>
-      <c r="I3" t="s" s="8">
-        <v>37</v>
-      </c>
-      <c r="J3" t="s" s="8">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="s" s="8">
-        <v>1264</v>
-      </c>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
-      <c r="D4" t="s" s="8">
-        <v>1265</v>
-      </c>
-      <c r="E4" t="s" s="8">
-        <v>1268</v>
-      </c>
-      <c r="F4" t="s" s="24">
-        <v>750</v>
-      </c>
-      <c r="G4" t="s" s="24">
-        <v>751</v>
-      </c>
-      <c r="H4" t="s" s="8">
-        <v>752</v>
-      </c>
-      <c r="I4" t="s" s="8">
-        <v>37</v>
-      </c>
-      <c r="J4" t="s" s="8">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s" s="8">
-        <v>1264</v>
-      </c>
-      <c r="B5" s="8"/>
-      <c r="C5" s="8"/>
-      <c r="D5" t="s" s="8">
-        <v>1265</v>
-      </c>
-      <c r="E5" t="s" s="8">
-        <v>1269</v>
-      </c>
-      <c r="F5" t="s" s="24">
-        <v>758</v>
-      </c>
-      <c r="G5" t="s" s="24">
-        <v>759</v>
-      </c>
-      <c r="H5" t="s" s="8">
-        <v>760</v>
-      </c>
-      <c r="I5" t="s" s="8">
-        <v>37</v>
-      </c>
-      <c r="J5" t="s" s="8">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s" s="8">
-        <v>1270</v>
-      </c>
-      <c r="B6" s="8" t="n">
-        <v>21.0</v>
-      </c>
-      <c r="C6" s="8"/>
-      <c r="D6" t="s" s="8">
-        <v>1271</v>
-      </c>
-      <c r="E6" t="s" s="8">
-        <v>1272</v>
-      </c>
-      <c r="F6" t="s" s="24">
-        <v>1149</v>
-      </c>
-      <c r="G6" t="s" s="24">
-        <v>1150</v>
-      </c>
-      <c r="H6" t="s" s="8">
-        <v>1151</v>
-      </c>
-      <c r="I6" t="s" s="8">
-        <v>51</v>
-      </c>
-      <c r="J6" t="s" s="8">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="s" s="8">
-        <v>1270</v>
-      </c>
-      <c r="B7" s="8" t="n">
-        <v>39.0</v>
-      </c>
-      <c r="C7" s="8"/>
-      <c r="D7" t="s" s="8">
-        <v>1271</v>
-      </c>
-      <c r="E7" t="s" s="8">
-        <v>1272</v>
-      </c>
-      <c r="F7" t="s" s="8">
-        <v>1149</v>
-      </c>
-      <c r="G7" t="s" s="8">
-        <v>1150</v>
-      </c>
-      <c r="H7" t="s" s="8">
-        <v>1151</v>
-      </c>
-      <c r="I7" t="s" s="8">
-        <v>51</v>
-      </c>
-      <c r="J7" t="s" s="8">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="s" s="8">
-        <v>1270</v>
-      </c>
-      <c r="B8" s="8" t="n">
-        <v>70.0</v>
-      </c>
-      <c r="C8" s="8"/>
-      <c r="D8" t="s" s="8">
-        <v>1271</v>
-      </c>
-      <c r="E8" t="s" s="8">
-        <v>1272</v>
-      </c>
-      <c r="F8" t="s" s="8">
-        <v>1149</v>
-      </c>
-      <c r="G8" t="s" s="8">
-        <v>1150</v>
-      </c>
-      <c r="H8" t="s" s="8">
-        <v>1151</v>
-      </c>
-      <c r="I8" t="s" s="8">
-        <v>51</v>
-      </c>
-      <c r="J8" t="s" s="8">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="s" s="8">
-        <v>1270</v>
-      </c>
-      <c r="B9" s="8" t="n">
-        <v>114.0</v>
-      </c>
-      <c r="C9" s="8"/>
-      <c r="D9" t="s" s="8">
-        <v>1271</v>
-      </c>
-      <c r="E9" t="s" s="8">
-        <v>1272</v>
-      </c>
-      <c r="F9" t="s" s="8">
-        <v>1149</v>
-      </c>
-      <c r="G9" t="s" s="8">
-        <v>1150</v>
-      </c>
-      <c r="H9" t="s" s="8">
-        <v>1151</v>
-      </c>
-      <c r="I9" t="s" s="8">
-        <v>51</v>
-      </c>
-      <c r="J9" t="s" s="8">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="s" s="8">
-        <v>1270</v>
-      </c>
-      <c r="B10" s="8" t="n">
-        <v>138.0</v>
-      </c>
-      <c r="C10" s="8"/>
-      <c r="D10" t="s" s="8">
-        <v>1271</v>
-      </c>
-      <c r="E10" t="s" s="8">
-        <v>1272</v>
-      </c>
-      <c r="F10" t="s" s="8">
-        <v>1149</v>
-      </c>
-      <c r="G10" t="s" s="8">
-        <v>1150</v>
-      </c>
-      <c r="H10" t="s" s="8">
-        <v>1151</v>
-      </c>
-      <c r="I10" t="s" s="8">
-        <v>51</v>
-      </c>
-      <c r="J10" t="s" s="8">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="s" s="8">
-        <v>1270</v>
-      </c>
-      <c r="B11" s="8" t="n">
-        <v>140.0</v>
-      </c>
-      <c r="C11" s="8"/>
-      <c r="D11" t="s" s="8">
-        <v>1271</v>
-      </c>
-      <c r="E11" t="s" s="8">
-        <v>1272</v>
-      </c>
-      <c r="F11" t="s" s="8">
-        <v>1149</v>
-      </c>
-      <c r="G11" t="s" s="8">
-        <v>1150</v>
-      </c>
-      <c r="H11" t="s" s="8">
-        <v>1151</v>
-      </c>
-      <c r="I11" t="s" s="8">
-        <v>51</v>
-      </c>
-      <c r="J11" t="s" s="8">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="s" s="8">
-        <v>1270</v>
-      </c>
-      <c r="B12" s="8" t="n">
-        <v>154.0</v>
-      </c>
-      <c r="C12" s="8"/>
-      <c r="D12" t="s" s="8">
-        <v>1271</v>
-      </c>
-      <c r="E12" t="s" s="8">
-        <v>1272</v>
-      </c>
-      <c r="F12" t="s" s="8">
-        <v>1149</v>
-      </c>
-      <c r="G12" t="s" s="8">
-        <v>1150</v>
-      </c>
-      <c r="H12" t="s" s="8">
-        <v>1151</v>
-      </c>
-      <c r="I12" t="s" s="8">
-        <v>51</v>
-      </c>
-      <c r="J12" t="s" s="8">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="s" s="8">
-        <v>1270</v>
-      </c>
-      <c r="B13" s="8" t="n">
-        <v>178.0</v>
-      </c>
-      <c r="C13" s="8"/>
-      <c r="D13" t="s" s="8">
-        <v>1271</v>
-      </c>
-      <c r="E13" t="s" s="8">
-        <v>1272</v>
-      </c>
-      <c r="F13" t="s" s="8">
-        <v>1149</v>
-      </c>
-      <c r="G13" t="s" s="8">
-        <v>1150</v>
-      </c>
-      <c r="H13" t="s" s="8">
-        <v>1151</v>
-      </c>
-      <c r="I13" t="s" s="8">
-        <v>51</v>
-      </c>
-      <c r="J13" t="s" s="8">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="s" s="8">
-        <v>1270</v>
-      </c>
-      <c r="B14" s="8" t="n">
-        <v>180.0</v>
-      </c>
-      <c r="C14" s="8"/>
-      <c r="D14" t="s" s="8">
-        <v>1271</v>
-      </c>
-      <c r="E14" t="s" s="8">
-        <v>1272</v>
-      </c>
-      <c r="F14" t="s" s="8">
-        <v>1149</v>
-      </c>
-      <c r="G14" t="s" s="8">
-        <v>1150</v>
-      </c>
-      <c r="H14" t="s" s="8">
-        <v>1151</v>
-      </c>
-      <c r="I14" t="s" s="8">
-        <v>51</v>
-      </c>
-      <c r="J14" t="s" s="8">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="s" s="8">
-        <v>1270</v>
-      </c>
-      <c r="B15" s="8" t="n">
-        <v>230.0</v>
-      </c>
-      <c r="C15" s="8"/>
-      <c r="D15" t="s" s="8">
-        <v>1271</v>
-      </c>
-      <c r="E15" t="s" s="8">
-        <v>1272</v>
-      </c>
-      <c r="F15" t="s" s="8">
-        <v>1149</v>
-      </c>
-      <c r="G15" t="s" s="8">
-        <v>1150</v>
-      </c>
-      <c r="H15" t="s" s="8">
-        <v>1151</v>
-      </c>
-      <c r="I15" t="s" s="8">
-        <v>51</v>
-      </c>
-      <c r="J15" t="s" s="8">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="s" s="8">
-        <v>1270</v>
-      </c>
-      <c r="B16" s="8" t="n">
-        <v>245.0</v>
-      </c>
-      <c r="C16" s="8"/>
-      <c r="D16" t="s" s="8">
-        <v>1271</v>
-      </c>
-      <c r="E16" t="s" s="8">
-        <v>1272</v>
-      </c>
-      <c r="F16" t="s" s="8">
-        <v>1149</v>
-      </c>
-      <c r="G16" t="s" s="8">
-        <v>1150</v>
-      </c>
-      <c r="H16" t="s" s="8">
-        <v>1151</v>
-      </c>
-      <c r="I16" t="s" s="8">
-        <v>51</v>
-      </c>
-      <c r="J16" t="s" s="8">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="s" s="8">
-        <v>1270</v>
-      </c>
-      <c r="B17" s="8" t="n">
-        <v>261.0</v>
-      </c>
-      <c r="C17" s="8"/>
-      <c r="D17" t="s" s="8">
-        <v>1271</v>
-      </c>
-      <c r="E17" t="s" s="8">
-        <v>1272</v>
-      </c>
-      <c r="F17" t="s" s="8">
-        <v>1149</v>
-      </c>
-      <c r="G17" t="s" s="8">
-        <v>1150</v>
-      </c>
-      <c r="H17" t="s" s="8">
-        <v>1151</v>
-      </c>
-      <c r="I17" t="s" s="8">
-        <v>51</v>
-      </c>
-      <c r="J17" t="s" s="8">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="s" s="8">
-        <v>1273</v>
-      </c>
-      <c r="B18" s="8"/>
-      <c r="C18" s="8"/>
-      <c r="D18" t="s" s="8">
-        <v>1274</v>
-      </c>
-      <c r="E18" t="s" s="8">
-        <v>1275</v>
-      </c>
-      <c r="F18" t="s" s="24">
-        <v>634</v>
-      </c>
-      <c r="G18" t="s" s="24">
-        <v>635</v>
-      </c>
-      <c r="H18" t="s" s="8">
-        <v>636</v>
-      </c>
-      <c r="I18" t="s" s="8">
-        <v>249</v>
-      </c>
-      <c r="J18" t="s" s="8">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="s" s="8">
-        <v>1273</v>
-      </c>
-      <c r="B19" s="8"/>
-      <c r="C19" s="8"/>
-      <c r="D19" t="s" s="8">
-        <v>1274</v>
-      </c>
-      <c r="E19" t="s" s="8">
-        <v>1276</v>
-      </c>
-      <c r="F19" t="s" s="8">
-        <v>634</v>
-      </c>
-      <c r="G19" t="s" s="8">
-        <v>635</v>
-      </c>
-      <c r="H19" t="s" s="8">
-        <v>636</v>
-      </c>
-      <c r="I19" t="s" s="8">
-        <v>249</v>
-      </c>
-      <c r="J19" t="s" s="8">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="s" s="8">
-        <v>1273</v>
-      </c>
-      <c r="B20" s="8"/>
-      <c r="C20" s="8"/>
-      <c r="D20" t="s" s="8">
-        <v>1274</v>
-      </c>
-      <c r="E20" t="s" s="8">
-        <v>1277</v>
-      </c>
-      <c r="F20" t="s" s="8">
-        <v>634</v>
-      </c>
-      <c r="G20" t="s" s="8">
-        <v>635</v>
-      </c>
-      <c r="H20" t="s" s="8">
-        <v>636</v>
-      </c>
-      <c r="I20" t="s" s="8">
-        <v>249</v>
-      </c>
-      <c r="J20" t="s" s="8">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="s" s="8">
-        <v>1273</v>
-      </c>
-      <c r="B21" s="8" t="n">
-        <v>371.0</v>
-      </c>
-      <c r="C21" s="8"/>
-      <c r="D21" t="s" s="8">
-        <v>1278</v>
-      </c>
-      <c r="E21" t="s" s="8">
-        <v>1279</v>
-      </c>
-      <c r="F21" t="s" s="24">
-        <v>666</v>
-      </c>
-      <c r="G21" t="s" s="24">
-        <v>667</v>
-      </c>
-      <c r="H21" t="s" s="8">
-        <v>1280</v>
-      </c>
-      <c r="I21" t="s" s="8">
-        <v>37</v>
-      </c>
-      <c r="J21" t="s" s="8">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="s" s="8">
-        <v>1281</v>
-      </c>
-      <c r="B22" s="8"/>
-      <c r="C22" s="8" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="D22" t="s" s="8">
-        <v>1282</v>
-      </c>
-      <c r="E22" t="s" s="8">
-        <v>1283</v>
-      </c>
-      <c r="F22" t="s" s="24">
-        <v>12</v>
-      </c>
-      <c r="G22" t="s" s="24">
-        <v>13</v>
-      </c>
-      <c r="H22" t="s" s="8">
-        <v>1284</v>
-      </c>
-      <c r="I22" t="s" s="8">
-        <v>10</v>
-      </c>
-      <c r="J22" t="s" s="8">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="s" s="8">
-        <v>1281</v>
-      </c>
-      <c r="B23" s="8"/>
-      <c r="C23" s="8" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="D23" t="s" s="8">
-        <v>1285</v>
-      </c>
-      <c r="E23" t="s" s="8">
-        <v>1286</v>
-      </c>
-      <c r="F23" t="s" s="24">
-        <v>12</v>
-      </c>
-      <c r="G23" t="s" s="24">
-        <v>13</v>
-      </c>
-      <c r="H23" t="s" s="8">
-        <v>1287</v>
-      </c>
-      <c r="I23" t="s" s="8">
-        <v>10</v>
-      </c>
-      <c r="J23" t="s" s="8">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="s" s="8">
-        <v>1288</v>
-      </c>
-      <c r="B24" s="8"/>
-      <c r="C24" s="8"/>
-      <c r="D24" t="s" s="8">
-        <v>1274</v>
-      </c>
-      <c r="E24" t="s" s="8">
-        <v>1289</v>
-      </c>
-      <c r="F24" t="s" s="24">
-        <v>634</v>
-      </c>
-      <c r="G24" t="s" s="24">
-        <v>635</v>
-      </c>
-      <c r="H24" t="s" s="8">
-        <v>636</v>
-      </c>
-      <c r="I24" t="s" s="8">
-        <v>249</v>
-      </c>
-      <c r="J24" t="s" s="8">
-        <v>16</v>
-      </c>
-    </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink location="'Rules'!A184" ref="F2"/>
-    <hyperlink location="'Rules'!A184" ref="G2"/>
-    <hyperlink location="'Rules'!A185" ref="F3"/>
-    <hyperlink location="'Rules'!A185" ref="G3"/>
-    <hyperlink location="'Rules'!A187" ref="F4"/>
-    <hyperlink location="'Rules'!A187" ref="G4"/>
-    <hyperlink location="'Rules'!A189" ref="F5"/>
-    <hyperlink location="'Rules'!A189" ref="G5"/>
-    <hyperlink location="'Rules'!A287" ref="F6"/>
-    <hyperlink location="'Rules'!A287" ref="G6"/>
-    <hyperlink location="'Rules'!A158" ref="F18"/>
-    <hyperlink location="'Rules'!A158" ref="G18"/>
-    <hyperlink location="'Rules'!A166" ref="F21"/>
-    <hyperlink location="'Rules'!A166" ref="G21"/>
-    <hyperlink location="'Rules'!A3" ref="F22"/>
-    <hyperlink location="'Rules'!A3" ref="G22"/>
-    <hyperlink location="'Rules'!A3" ref="F23"/>
-    <hyperlink location="'Rules'!A3" ref="G23"/>
-    <hyperlink location="'Rules'!A158" ref="F24"/>
-    <hyperlink location="'Rules'!A158" ref="G24"/>
-  </hyperlinks>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>

</xml_diff>